<commit_message>
update meta to include renewables and exclude consumer data transfer
</commit_message>
<xml_diff>
--- a/data/companies/meta/MetaCorporate.xlsx
+++ b/data/companies/meta/MetaCorporate.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://scopethree-my.sharepoint.com/personal/rlissack_scope3_com/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bokelley/src/methodology/data/companies/meta/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{64BEB9D9-984C-4C57-A26C-B1B35EE0CA06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0F543C8-86AE-7448-9D51-A7364ED3A8A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1360" yWindow="880" windowWidth="26840" windowHeight="15940" xr2:uid="{B9EE70E7-5244-0C4E-83EB-F407CD4AECF2}"/>
+    <workbookView xWindow="4140" yWindow="2300" windowWidth="26840" windowHeight="15940" xr2:uid="{B9EE70E7-5244-0C4E-83EB-F407CD4AECF2}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Corporate assessment" sheetId="1" r:id="rId1"/>
+    <sheet name="Properties" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="47">
   <si>
     <t>Facts</t>
   </si>
@@ -62,12 +63,6 @@
     <t>Location</t>
   </si>
   <si>
-    <t>Scope 2 market based</t>
-  </si>
-  <si>
-    <t>(plus) Scope 2 location based</t>
-  </si>
-  <si>
     <t xml:space="preserve">I - pg 1 </t>
   </si>
   <si>
@@ -77,42 +72,18 @@
     <t>Meta-10K</t>
   </si>
   <si>
-    <t>Page 70</t>
-  </si>
-  <si>
-    <t>Scope 3 total using (market)</t>
-  </si>
-  <si>
     <t>D</t>
   </si>
   <si>
     <t>Meta sustainability</t>
   </si>
   <si>
-    <t>page 50</t>
-  </si>
-  <si>
-    <t>(plus) Scope 3 location based</t>
-  </si>
-  <si>
     <t>I</t>
   </si>
   <si>
     <t>Meta Sustainability Auditor Statement 2021</t>
   </si>
   <si>
-    <t xml:space="preserve">Page 1 </t>
-  </si>
-  <si>
-    <t>Renewable Energy PPA</t>
-  </si>
-  <si>
-    <t>Renewable Offsets</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I-pg 2 </t>
-  </si>
-  <si>
     <t>(minus) Carbon Credits that meet CAC std</t>
   </si>
   <si>
@@ -137,16 +108,76 @@
     <t>Apps (FB/IG/WhatsApp)</t>
   </si>
   <si>
-    <t>Location based Emissions</t>
-  </si>
-  <si>
-    <t>Location based Total Emission - GHG Offsets</t>
-  </si>
-  <si>
     <t>mtC02e/employee</t>
   </si>
   <si>
     <t>mtC02e/$MTotalRevenue</t>
+  </si>
+  <si>
+    <t>Property</t>
+  </si>
+  <si>
+    <t>% of corporate emissions</t>
+  </si>
+  <si>
+    <t>Facebook</t>
+  </si>
+  <si>
+    <t>Instagram</t>
+  </si>
+  <si>
+    <t>% ad supported</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Other - not ad supported</t>
+  </si>
+  <si>
+    <t>Net location-based emissions</t>
+  </si>
+  <si>
+    <t>Not clearly documentated but giving benefit of doubt</t>
+  </si>
+  <si>
+    <t>D - pg 51</t>
+  </si>
+  <si>
+    <t>D - pg 50,52</t>
+  </si>
+  <si>
+    <t>"selecting projects that are on the same energy grids as our data centers"</t>
+  </si>
+  <si>
+    <t>(plus) Scope 2 market based</t>
+  </si>
+  <si>
+    <t>Scope 2 location based</t>
+  </si>
+  <si>
+    <t>(plus) Scope 3 total using (market)</t>
+  </si>
+  <si>
+    <t>(minus) Scope 3 consumer device</t>
+  </si>
+  <si>
+    <t>Using market per qualified renewable methodology</t>
+  </si>
+  <si>
+    <t>Allocated net emissions</t>
+  </si>
+  <si>
+    <t>(plus) adjustment for embodied emissions</t>
+  </si>
+  <si>
+    <t>J</t>
+  </si>
+  <si>
+    <t>Environmental Metrics Methodology</t>
+  </si>
+  <si>
+    <t>LCA includes upfront emissions from office renovations, new construction, datacenters, and hardware. Possibly omits some hardware components.</t>
   </si>
 </sst>
 </file>
@@ -160,7 +191,7 @@
     <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -191,6 +222,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -200,7 +239,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -208,14 +247,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -225,12 +274,20 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="4" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="4" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Currency" xfId="2" builtinId="4"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="4" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -542,20 +599,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5792829F-E540-1242-9E1B-7377B1C9ECB9}">
-  <dimension ref="A1:J21"/>
+  <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="A19" sqref="A19:D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="34.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.6640625" customWidth="1"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="34.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -567,8 +625,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
-      <c r="A2" t="s">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="9" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="2">
@@ -580,16 +638,10 @@
       <c r="D2" t="s">
         <v>5</v>
       </c>
-      <c r="H2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3" t="s">
-        <v>8</v>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="9" t="s">
+        <v>37</v>
       </c>
       <c r="B3" s="2">
         <v>2000</v>
@@ -598,13 +650,15 @@
         <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>5</v>
-      </c>
-      <c r="I3" s="7"/>
-    </row>
-    <row r="4" spans="1:10">
+        <v>35</v>
+      </c>
+      <c r="E3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>38</v>
       </c>
       <c r="B4" s="2">
         <v>3080194</v>
@@ -613,21 +667,15 @@
         <v>4</v>
       </c>
       <c r="D4" t="s">
-        <v>10</v>
-      </c>
-      <c r="H4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I4" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="J4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5" t="s">
-        <v>14</v>
+        <v>8</v>
+      </c>
+      <c r="E4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="9" t="s">
+        <v>39</v>
       </c>
       <c r="B5" s="2">
         <v>5651000</v>
@@ -635,43 +683,46 @@
       <c r="C5" t="s">
         <v>4</v>
       </c>
-      <c r="H5" t="s">
-        <v>15</v>
-      </c>
-      <c r="I5" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="J5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" t="s">
-        <v>18</v>
+      <c r="D5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="9" t="s">
+        <v>40</v>
       </c>
       <c r="B6" s="2">
-        <v>9900000</v>
+        <f>558000</f>
+        <v>558000</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
       </c>
-      <c r="H6" t="s">
-        <v>19</v>
-      </c>
-      <c r="I6" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="J6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="B7" s="2"/>
+      <c r="D6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="2">
+        <v>90000</v>
+      </c>
+      <c r="C7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" t="s">
+        <v>33</v>
+      </c>
       <c r="I7" s="7"/>
     </row>
-    <row r="8" spans="1:10">
-      <c r="A8" t="s">
-        <v>22</v>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="9" t="s">
+        <v>43</v>
       </c>
       <c r="B8" s="2">
         <v>0</v>
@@ -679,116 +730,228 @@
       <c r="C8" t="s">
         <v>4</v>
       </c>
+      <c r="D8" t="s">
+        <v>44</v>
+      </c>
+      <c r="E8" t="s">
+        <v>46</v>
+      </c>
       <c r="I8" s="7"/>
     </row>
-    <row r="9" spans="1:10">
-      <c r="A9" t="s">
-        <v>23</v>
-      </c>
-      <c r="B9" s="2">
-        <v>90000</v>
-      </c>
-      <c r="C9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D9" t="s">
-        <v>24</v>
-      </c>
-      <c r="I9" s="7"/>
-    </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>25</v>
-      </c>
-      <c r="B10" s="2">
-        <v>90000</v>
-      </c>
-      <c r="C10" t="s">
-        <v>4</v>
-      </c>
-      <c r="I10" s="7"/>
-    </row>
-    <row r="12" spans="1:10">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="8">
+        <v>86482</v>
+      </c>
+      <c r="D11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10">
+        <v>19</v>
+      </c>
+      <c r="B12" s="3">
+        <v>117929</v>
+      </c>
+      <c r="C12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>27</v>
-      </c>
-      <c r="B13" s="8">
-        <v>86482</v>
-      </c>
-      <c r="D13" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10">
-      <c r="A14" t="s">
-        <v>29</v>
-      </c>
-      <c r="B14" s="3">
-        <v>117929</v>
-      </c>
-      <c r="C14" t="s">
-        <v>30</v>
-      </c>
-      <c r="D14" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10">
+        <v>22</v>
+      </c>
+      <c r="B13" s="3">
+        <v>115655</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>32</v>
       </c>
-      <c r="B15" s="3">
-        <v>115655</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
+      <c r="B15" s="4">
+        <f>B2+B3+B5-B6-B7</f>
+        <v>5060000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" s="5">
+        <f>B15/B11</f>
+        <v>58.509285169168152</v>
+      </c>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>33</v>
-      </c>
-      <c r="B17" s="4">
-        <f>B2+B4+B6-B10</f>
-        <v>12945194</v>
-      </c>
-      <c r="D17" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" t="s">
-        <v>35</v>
-      </c>
-      <c r="B18" s="5">
-        <f>B17/B13</f>
-        <v>149.68657061585068</v>
-      </c>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" t="s">
-        <v>36</v>
-      </c>
-      <c r="B19" s="6">
-        <f>B17/B14</f>
-        <v>109.77108260054779</v>
-      </c>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="B21" s="2"/>
+        <v>24</v>
+      </c>
+      <c r="B17" s="6">
+        <f>B15/B12</f>
+        <v>42.907172960001354</v>
+      </c>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>27</v>
+      </c>
+      <c r="B20" s="12">
+        <v>0.38</v>
+      </c>
+      <c r="C20" s="14">
+        <v>1</v>
+      </c>
+      <c r="D20" s="4">
+        <f>$B$15*B20*C20</f>
+        <v>1922800</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21" s="12">
+        <v>0.44</v>
+      </c>
+      <c r="C21" s="14">
+        <v>1</v>
+      </c>
+      <c r="D21" s="4">
+        <f t="shared" ref="D21:D22" si="0">$B$15*B21*C21</f>
+        <v>2226400</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B22" s="13">
+        <f>1-SUM(B20:B21)</f>
+        <v>0.17999999999999994</v>
+      </c>
+      <c r="C22" s="15">
+        <v>0</v>
+      </c>
+      <c r="D22" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23" s="14">
+        <f>SUM(B20:B22)</f>
+        <v>1</v>
+      </c>
+      <c r="D23" s="4">
+        <f>SUM(D20:D22)</f>
+        <v>4149200</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B24" s="2"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B31" s="7"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>9</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>11</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>13</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>44</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>45</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="I4" r:id="rId1" xr:uid="{93C17B07-9D5A-9F47-B617-130C718BDC1C}"/>
-    <hyperlink ref="I5" r:id="rId2" xr:uid="{8D616ED0-F2B8-2142-8E71-D148A1E5BF07}"/>
-    <hyperlink ref="I6" r:id="rId3" xr:uid="{3375467A-9679-BD43-830C-91C3FE923EFD}"/>
+    <hyperlink ref="B32" r:id="rId1" xr:uid="{93C17B07-9D5A-9F47-B617-130C718BDC1C}"/>
+    <hyperlink ref="B33" r:id="rId2" xr:uid="{8D616ED0-F2B8-2142-8E71-D148A1E5BF07}"/>
+    <hyperlink ref="B34" r:id="rId3" xr:uid="{3375467A-9679-BD43-830C-91C3FE923EFD}"/>
+    <hyperlink ref="B35" r:id="rId4" xr:uid="{7A3375A1-BDF0-6B43-B172-E6FD7E8A6267}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D03ED8A-A375-B24B-BA33-89C2A1087CDC}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="21.1640625" customWidth="1"/>
+    <col min="2" max="2" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.5" customWidth="1"/>
+  </cols>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
update meta to include renewables and exclude consumer data transfer (#113)
* update meta to include renewables and exclude consumer data transfer

* update defaults files.
reran the cli/compute_defaults.py to take into account Meta consumer device
emissions.

---------

Co-authored-by: Ron Lissack <rlissack@scope3.com>
</commit_message>
<xml_diff>
--- a/data/companies/meta/MetaCorporate.xlsx
+++ b/data/companies/meta/MetaCorporate.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://scopethree-my.sharepoint.com/personal/rlissack_scope3_com/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bokelley/src/methodology/data/companies/meta/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{64BEB9D9-984C-4C57-A26C-B1B35EE0CA06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0F543C8-86AE-7448-9D51-A7364ED3A8A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1360" yWindow="880" windowWidth="26840" windowHeight="15940" xr2:uid="{B9EE70E7-5244-0C4E-83EB-F407CD4AECF2}"/>
+    <workbookView xWindow="4140" yWindow="2300" windowWidth="26840" windowHeight="15940" xr2:uid="{B9EE70E7-5244-0C4E-83EB-F407CD4AECF2}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Corporate assessment" sheetId="1" r:id="rId1"/>
+    <sheet name="Properties" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="47">
   <si>
     <t>Facts</t>
   </si>
@@ -62,12 +63,6 @@
     <t>Location</t>
   </si>
   <si>
-    <t>Scope 2 market based</t>
-  </si>
-  <si>
-    <t>(plus) Scope 2 location based</t>
-  </si>
-  <si>
     <t xml:space="preserve">I - pg 1 </t>
   </si>
   <si>
@@ -77,42 +72,18 @@
     <t>Meta-10K</t>
   </si>
   <si>
-    <t>Page 70</t>
-  </si>
-  <si>
-    <t>Scope 3 total using (market)</t>
-  </si>
-  <si>
     <t>D</t>
   </si>
   <si>
     <t>Meta sustainability</t>
   </si>
   <si>
-    <t>page 50</t>
-  </si>
-  <si>
-    <t>(plus) Scope 3 location based</t>
-  </si>
-  <si>
     <t>I</t>
   </si>
   <si>
     <t>Meta Sustainability Auditor Statement 2021</t>
   </si>
   <si>
-    <t xml:space="preserve">Page 1 </t>
-  </si>
-  <si>
-    <t>Renewable Energy PPA</t>
-  </si>
-  <si>
-    <t>Renewable Offsets</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I-pg 2 </t>
-  </si>
-  <si>
     <t>(minus) Carbon Credits that meet CAC std</t>
   </si>
   <si>
@@ -137,16 +108,76 @@
     <t>Apps (FB/IG/WhatsApp)</t>
   </si>
   <si>
-    <t>Location based Emissions</t>
-  </si>
-  <si>
-    <t>Location based Total Emission - GHG Offsets</t>
-  </si>
-  <si>
     <t>mtC02e/employee</t>
   </si>
   <si>
     <t>mtC02e/$MTotalRevenue</t>
+  </si>
+  <si>
+    <t>Property</t>
+  </si>
+  <si>
+    <t>% of corporate emissions</t>
+  </si>
+  <si>
+    <t>Facebook</t>
+  </si>
+  <si>
+    <t>Instagram</t>
+  </si>
+  <si>
+    <t>% ad supported</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Other - not ad supported</t>
+  </si>
+  <si>
+    <t>Net location-based emissions</t>
+  </si>
+  <si>
+    <t>Not clearly documentated but giving benefit of doubt</t>
+  </si>
+  <si>
+    <t>D - pg 51</t>
+  </si>
+  <si>
+    <t>D - pg 50,52</t>
+  </si>
+  <si>
+    <t>"selecting projects that are on the same energy grids as our data centers"</t>
+  </si>
+  <si>
+    <t>(plus) Scope 2 market based</t>
+  </si>
+  <si>
+    <t>Scope 2 location based</t>
+  </si>
+  <si>
+    <t>(plus) Scope 3 total using (market)</t>
+  </si>
+  <si>
+    <t>(minus) Scope 3 consumer device</t>
+  </si>
+  <si>
+    <t>Using market per qualified renewable methodology</t>
+  </si>
+  <si>
+    <t>Allocated net emissions</t>
+  </si>
+  <si>
+    <t>(plus) adjustment for embodied emissions</t>
+  </si>
+  <si>
+    <t>J</t>
+  </si>
+  <si>
+    <t>Environmental Metrics Methodology</t>
+  </si>
+  <si>
+    <t>LCA includes upfront emissions from office renovations, new construction, datacenters, and hardware. Possibly omits some hardware components.</t>
   </si>
 </sst>
 </file>
@@ -160,7 +191,7 @@
     <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -191,6 +222,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -200,7 +239,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -208,14 +247,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -225,12 +274,20 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="4" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="4" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Currency" xfId="2" builtinId="4"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="4" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -542,20 +599,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5792829F-E540-1242-9E1B-7377B1C9ECB9}">
-  <dimension ref="A1:J21"/>
+  <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="A19" sqref="A19:D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="34.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.6640625" customWidth="1"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="34.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -567,8 +625,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
-      <c r="A2" t="s">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="9" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="2">
@@ -580,16 +638,10 @@
       <c r="D2" t="s">
         <v>5</v>
       </c>
-      <c r="H2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3" t="s">
-        <v>8</v>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="9" t="s">
+        <v>37</v>
       </c>
       <c r="B3" s="2">
         <v>2000</v>
@@ -598,13 +650,15 @@
         <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>5</v>
-      </c>
-      <c r="I3" s="7"/>
-    </row>
-    <row r="4" spans="1:10">
+        <v>35</v>
+      </c>
+      <c r="E3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>38</v>
       </c>
       <c r="B4" s="2">
         <v>3080194</v>
@@ -613,21 +667,15 @@
         <v>4</v>
       </c>
       <c r="D4" t="s">
-        <v>10</v>
-      </c>
-      <c r="H4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I4" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="J4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5" t="s">
-        <v>14</v>
+        <v>8</v>
+      </c>
+      <c r="E4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="9" t="s">
+        <v>39</v>
       </c>
       <c r="B5" s="2">
         <v>5651000</v>
@@ -635,43 +683,46 @@
       <c r="C5" t="s">
         <v>4</v>
       </c>
-      <c r="H5" t="s">
-        <v>15</v>
-      </c>
-      <c r="I5" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="J5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" t="s">
-        <v>18</v>
+      <c r="D5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="9" t="s">
+        <v>40</v>
       </c>
       <c r="B6" s="2">
-        <v>9900000</v>
+        <f>558000</f>
+        <v>558000</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
       </c>
-      <c r="H6" t="s">
-        <v>19</v>
-      </c>
-      <c r="I6" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="J6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="B7" s="2"/>
+      <c r="D6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="2">
+        <v>90000</v>
+      </c>
+      <c r="C7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" t="s">
+        <v>33</v>
+      </c>
       <c r="I7" s="7"/>
     </row>
-    <row r="8" spans="1:10">
-      <c r="A8" t="s">
-        <v>22</v>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="9" t="s">
+        <v>43</v>
       </c>
       <c r="B8" s="2">
         <v>0</v>
@@ -679,116 +730,228 @@
       <c r="C8" t="s">
         <v>4</v>
       </c>
+      <c r="D8" t="s">
+        <v>44</v>
+      </c>
+      <c r="E8" t="s">
+        <v>46</v>
+      </c>
       <c r="I8" s="7"/>
     </row>
-    <row r="9" spans="1:10">
-      <c r="A9" t="s">
-        <v>23</v>
-      </c>
-      <c r="B9" s="2">
-        <v>90000</v>
-      </c>
-      <c r="C9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D9" t="s">
-        <v>24</v>
-      </c>
-      <c r="I9" s="7"/>
-    </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>25</v>
-      </c>
-      <c r="B10" s="2">
-        <v>90000</v>
-      </c>
-      <c r="C10" t="s">
-        <v>4</v>
-      </c>
-      <c r="I10" s="7"/>
-    </row>
-    <row r="12" spans="1:10">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="8">
+        <v>86482</v>
+      </c>
+      <c r="D11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10">
+        <v>19</v>
+      </c>
+      <c r="B12" s="3">
+        <v>117929</v>
+      </c>
+      <c r="C12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>27</v>
-      </c>
-      <c r="B13" s="8">
-        <v>86482</v>
-      </c>
-      <c r="D13" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10">
-      <c r="A14" t="s">
-        <v>29</v>
-      </c>
-      <c r="B14" s="3">
-        <v>117929</v>
-      </c>
-      <c r="C14" t="s">
-        <v>30</v>
-      </c>
-      <c r="D14" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10">
+        <v>22</v>
+      </c>
+      <c r="B13" s="3">
+        <v>115655</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>32</v>
       </c>
-      <c r="B15" s="3">
-        <v>115655</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
+      <c r="B15" s="4">
+        <f>B2+B3+B5-B6-B7</f>
+        <v>5060000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" s="5">
+        <f>B15/B11</f>
+        <v>58.509285169168152</v>
+      </c>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>33</v>
-      </c>
-      <c r="B17" s="4">
-        <f>B2+B4+B6-B10</f>
-        <v>12945194</v>
-      </c>
-      <c r="D17" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" t="s">
-        <v>35</v>
-      </c>
-      <c r="B18" s="5">
-        <f>B17/B13</f>
-        <v>149.68657061585068</v>
-      </c>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" t="s">
-        <v>36</v>
-      </c>
-      <c r="B19" s="6">
-        <f>B17/B14</f>
-        <v>109.77108260054779</v>
-      </c>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="B21" s="2"/>
+        <v>24</v>
+      </c>
+      <c r="B17" s="6">
+        <f>B15/B12</f>
+        <v>42.907172960001354</v>
+      </c>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>27</v>
+      </c>
+      <c r="B20" s="12">
+        <v>0.38</v>
+      </c>
+      <c r="C20" s="14">
+        <v>1</v>
+      </c>
+      <c r="D20" s="4">
+        <f>$B$15*B20*C20</f>
+        <v>1922800</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21" s="12">
+        <v>0.44</v>
+      </c>
+      <c r="C21" s="14">
+        <v>1</v>
+      </c>
+      <c r="D21" s="4">
+        <f t="shared" ref="D21:D22" si="0">$B$15*B21*C21</f>
+        <v>2226400</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B22" s="13">
+        <f>1-SUM(B20:B21)</f>
+        <v>0.17999999999999994</v>
+      </c>
+      <c r="C22" s="15">
+        <v>0</v>
+      </c>
+      <c r="D22" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23" s="14">
+        <f>SUM(B20:B22)</f>
+        <v>1</v>
+      </c>
+      <c r="D23" s="4">
+        <f>SUM(D20:D22)</f>
+        <v>4149200</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B24" s="2"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B31" s="7"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>9</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>11</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>13</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>44</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>45</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="I4" r:id="rId1" xr:uid="{93C17B07-9D5A-9F47-B617-130C718BDC1C}"/>
-    <hyperlink ref="I5" r:id="rId2" xr:uid="{8D616ED0-F2B8-2142-8E71-D148A1E5BF07}"/>
-    <hyperlink ref="I6" r:id="rId3" xr:uid="{3375467A-9679-BD43-830C-91C3FE923EFD}"/>
+    <hyperlink ref="B32" r:id="rId1" xr:uid="{93C17B07-9D5A-9F47-B617-130C718BDC1C}"/>
+    <hyperlink ref="B33" r:id="rId2" xr:uid="{8D616ED0-F2B8-2142-8E71-D148A1E5BF07}"/>
+    <hyperlink ref="B34" r:id="rId3" xr:uid="{3375467A-9679-BD43-830C-91C3FE923EFD}"/>
+    <hyperlink ref="B35" r:id="rId4" xr:uid="{7A3375A1-BDF0-6B43-B172-E6FD7E8A6267}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D03ED8A-A375-B24B-BA33-89C2A1087CDC}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="21.1640625" customWidth="1"/>
+    <col min="2" max="2" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.5" customWidth="1"/>
+  </cols>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>